<commit_message>
feat: user type class, started on sign in class
</commit_message>
<xml_diff>
--- a/test_data/test_data.xlsx
+++ b/test_data/test_data.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vsmyrnov\PycharmProjects\selenium-zgl-bvt\test_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2AF4851-A4B7-424D-A264-D277816E5393}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BFC7AC3-6E98-444C-9A5F-F41782DD3EC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2460" yWindow="945" windowWidth="26205" windowHeight="14235" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2460" yWindow="945" windowWidth="26205" windowHeight="14235" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Constants" sheetId="3" r:id="rId1"/>
     <sheet name="Meganav" sheetId="1" r:id="rId2"/>
     <sheet name="BVT" sheetId="2" r:id="rId3"/>
+    <sheet name="Users" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="80">
   <si>
     <t>Meganav Name</t>
   </si>
@@ -144,14 +145,145 @@
   </si>
   <si>
     <t>constant</t>
+  </si>
+  <si>
+    <t>user id</t>
+  </si>
+  <si>
+    <t>first name</t>
+  </si>
+  <si>
+    <t>last name</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>re password</t>
+  </si>
+  <si>
+    <t>phone</t>
+  </si>
+  <si>
+    <t>e2e-10</t>
+  </si>
+  <si>
+    <t>e2e-11</t>
+  </si>
+  <si>
+    <t>e2e-12</t>
+  </si>
+  <si>
+    <t>e2e-13</t>
+  </si>
+  <si>
+    <t>e2e-14</t>
+  </si>
+  <si>
+    <t>e2e-15</t>
+  </si>
+  <si>
+    <t>e2e-16</t>
+  </si>
+  <si>
+    <t>e2e-17</t>
+  </si>
+  <si>
+    <t>e2e-18</t>
+  </si>
+  <si>
+    <t>e2e-19</t>
+  </si>
+  <si>
+    <t>zgallerieautomation_tc10@zgqa.com</t>
+  </si>
+  <si>
+    <t>zgallerieautomation_tc11@zgqa.com</t>
+  </si>
+  <si>
+    <t>zgallerieautomation_tc12@zgqa.com</t>
+  </si>
+  <si>
+    <t>zgallerieautomation_tc13@zgqa.com</t>
+  </si>
+  <si>
+    <t>zgallerieautomation_tc14@zgqa.com</t>
+  </si>
+  <si>
+    <t>zgallerieautomation_tc15@zgqa.com</t>
+  </si>
+  <si>
+    <t>zgallerieautomation_tc16@zgqa.com</t>
+  </si>
+  <si>
+    <t>zgallerieautomation_tc17@zgqa.com</t>
+  </si>
+  <si>
+    <t>zgallerieautomation_tc18@zgqa.com</t>
+  </si>
+  <si>
+    <t>zgallerieautomation_tc19@zgqa.com</t>
+  </si>
+  <si>
+    <t>Password1</t>
+  </si>
+  <si>
+    <t>FIRST NAMES</t>
+  </si>
+  <si>
+    <t>['Johny', 'BahuBali', 'Sherlock', 'Ivan', 'Kassandra', 'Nefertiti']</t>
+  </si>
+  <si>
+    <t>LAST NAMES</t>
+  </si>
+  <si>
+    <t>['Holms',  'Batman', 'Karambulya', 'Dundar', 'Barmaley']</t>
+  </si>
+  <si>
+    <t>pay pal</t>
+  </si>
+  <si>
+    <t>jmatos@directbuy.com</t>
+  </si>
+  <si>
+    <t>draw~88~dress</t>
+  </si>
+  <si>
+    <t>random</t>
+  </si>
+  <si>
+    <t>Fname1</t>
+  </si>
+  <si>
+    <t>Lname1</t>
+  </si>
+  <si>
+    <t>Fname1@zgqa.com</t>
+  </si>
+  <si>
+    <t>new 1</t>
+  </si>
+  <si>
+    <t>new random</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
-    <font>
+  <fonts count="14" x14ac:knownFonts="1">
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -196,13 +328,76 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="11"/>
+      <color theme="9" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="5" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="11"/>
+      <color theme="5" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF002060"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="6" tint="-0.499984740745262"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="11"/>
+      <color theme="6" tint="-0.499984740745262"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -216,15 +411,24 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -506,16 +710,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F2B43D5-2FC5-4CCF-886B-08DFFA3DBD04}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13" customWidth="1"/>
-    <col min="2" max="2" width="42.42578125" customWidth="1"/>
+    <col min="2" max="2" width="54.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -532,6 +736,22 @@
       </c>
       <c r="B2" t="s">
         <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>67</v>
+      </c>
+      <c r="B3" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>69</v>
+      </c>
+      <c r="B4" t="s">
+        <v>70</v>
       </c>
     </row>
   </sheetData>
@@ -714,4 +934,275 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7544987D-61EB-40BF-AEE6-388E1D4A3981}">
+  <dimension ref="A1:G14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="34.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14" customWidth="1"/>
+    <col min="6" max="6" width="15.85546875" customWidth="1"/>
+    <col min="7" max="7" width="17.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="B11" s="3"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="B12" s="8"/>
+      <c r="C12" s="8"/>
+      <c r="D12" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="E12" s="8" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="B13" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="C13" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="D13" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="E13" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="F13" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="G13" s="10" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="B14" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="C14" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="D14" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="E14" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="F14" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="G14" s="10" t="s">
+        <v>74</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="7" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{144993FF-2F6C-49A9-9A1F-DDCB6807E14B}"/>
+    <hyperlink ref="D3" r:id="rId2" xr:uid="{C3F12CE7-B200-46A1-A74E-3FB3FD020297}"/>
+    <hyperlink ref="D4" r:id="rId3" xr:uid="{1A7C8710-D411-457B-83A9-4526A1CBE91B}"/>
+    <hyperlink ref="D6" r:id="rId4" xr:uid="{6673F2A9-1243-4C98-B6CF-AFC9D8036E04}"/>
+    <hyperlink ref="D8" r:id="rId5" xr:uid="{995A46BC-5B10-4EB1-80C9-4AEB6A54B765}"/>
+    <hyperlink ref="D10" r:id="rId6" xr:uid="{5F7C0A75-4924-46A9-AC1C-8CE8C35005FB}"/>
+    <hyperlink ref="D5" r:id="rId7" xr:uid="{BF610CEF-0892-42EF-9CF0-B84CA2EF4D14}"/>
+    <hyperlink ref="D7" r:id="rId8" xr:uid="{98FAD294-946E-44C2-B0EC-107676A06B68}"/>
+    <hyperlink ref="D9" r:id="rId9" xr:uid="{0B183D29-6919-4225-8648-6EFF74C00869}"/>
+    <hyperlink ref="D11" r:id="rId10" xr:uid="{6C99A9E9-1F71-4460-8B6D-96D531F7BC7E}"/>
+    <hyperlink ref="D12" r:id="rId11" xr:uid="{386AF918-E04F-4741-A52A-B4143C5DC082}"/>
+    <hyperlink ref="D14" r:id="rId12" xr:uid="{1FAA3988-47DB-405E-9C90-358C90309DB4}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>